<commit_message>
edit students button fixed
</commit_message>
<xml_diff>
--- a/StudentLists_data.xlsx
+++ b/StudentLists_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Injection</t>
   </si>
@@ -44,7 +44,7 @@
     <t>22100</t>
   </si>
   <si>
-    <t>anne</t>
+    <t>nosha</t>
   </si>
   <si>
     <t>17</t>
@@ -56,7 +56,7 @@
     <t>n@gmail.com</t>
   </si>
   <si>
-    <t>22100.0</t>
+    <t>22102</t>
   </si>
   <si>
     <t>6546.0</t>
@@ -74,30 +74,12 @@
     <t>d@gmail.com</t>
   </si>
   <si>
-    <t>22101.0</t>
+    <t>22101</t>
   </si>
   <si>
     <t>3555.0</t>
   </si>
   <si>
-    <t>lola</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>97898</t>
-  </si>
-  <si>
-    <t>l@gmail.com</t>
-  </si>
-  <si>
-    <t>22102.0</t>
-  </si>
-  <si>
-    <t>5466.0</t>
-  </si>
-  <si>
     <t>3li</t>
   </si>
   <si>
@@ -110,7 +92,7 @@
     <t>fhghf@g.com</t>
   </si>
   <si>
-    <t>22103.0</t>
+    <t>22103</t>
   </si>
   <si>
     <t>1234.0</t>
@@ -158,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -264,26 +246,6 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>